<commit_message>
Added AA uptake by Sbo, and two more metabolites
Also changed f() function kinetic block to update calculate and updated  bounds inside loops instead of having it hard coded
</commit_message>
<xml_diff>
--- a/iGEM simulation environment/GEMs/modelEre.xlsx
+++ b/iGEM simulation environment/GEMs/modelEre.xlsx
@@ -11794,7 +11794,7 @@
         <v>-1000.0</v>
       </c>
       <c r="H116" t="n" s="1">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="L116" t="s" s="1">
         <v>424</v>
@@ -11811,7 +11811,7 @@
         <v>448</v>
       </c>
       <c r="G117" t="n" s="1">
-        <v>-1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="H117" t="n" s="1">
         <v>1000.0</v>

</xml_diff>